<commit_message>
update spec and estimation (server side)
</commit_message>
<xml_diff>
--- a/document/Project Recipe Quotation.xlsx
+++ b/document/Project Recipe Quotation.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Login page</t>
   </si>
@@ -189,6 +189,24 @@
   </si>
   <si>
     <t>Profile page</t>
+  </si>
+  <si>
+    <t>Like function</t>
+  </si>
+  <si>
+    <t>Profile service</t>
+  </si>
+  <si>
+    <t>Comment service</t>
+  </si>
+  <si>
+    <t>Like service</t>
+  </si>
+  <si>
+    <t>Follow service</t>
+  </si>
+  <si>
+    <t>Feed Push Notification service</t>
   </si>
 </sst>
 </file>
@@ -375,7 +393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -410,6 +428,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -428,10 +450,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -756,7 +775,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.5" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="35" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -770,7 +789,7 @@
       <c r="G2" s="28"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="32"/>
+      <c r="A3" s="36"/>
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -784,7 +803,7 @@
       <c r="G3" s="27"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="32"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
@@ -798,7 +817,7 @@
       <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="32"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
@@ -812,7 +831,7 @@
       <c r="G5" s="27"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="32"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="6" t="s">
         <v>46</v>
       </c>
@@ -826,7 +845,7 @@
       <c r="G6" s="27"/>
     </row>
     <row r="7" spans="1:7" s="29" customFormat="1">
-      <c r="A7" s="32"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="6" t="s">
         <v>45</v>
       </c>
@@ -841,7 +860,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" s="29" customFormat="1">
-      <c r="A8" s="32"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="6" t="s">
         <v>48</v>
       </c>
@@ -849,12 +868,12 @@
         <v>4</v>
       </c>
       <c r="D8" s="10">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:7" s="29" customFormat="1">
-      <c r="A9" s="32"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
@@ -867,7 +886,7 @@
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:7" s="29" customFormat="1">
-      <c r="A10" s="32"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="6" t="s">
         <v>50</v>
       </c>
@@ -880,169 +899,171 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="32"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="37">
-        <v>4</v>
-      </c>
-      <c r="D11" s="38">
+      <c r="C11" s="31">
+        <v>4</v>
+      </c>
+      <c r="D11" s="32">
         <v>8</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="32"/>
       <c r="G11" s="27"/>
     </row>
     <row r="12" spans="1:7" s="29" customFormat="1">
-      <c r="A12" s="32"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="31">
+        <v>0</v>
+      </c>
+      <c r="D12" s="32">
+        <v>8</v>
+      </c>
+      <c r="E12" s="40"/>
+    </row>
+    <row r="13" spans="1:7" s="29" customFormat="1">
+      <c r="A13" s="36"/>
+      <c r="B13" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="7">
-        <v>4</v>
-      </c>
-      <c r="D12" s="8">
+      <c r="C13" s="7">
+        <v>4</v>
+      </c>
+      <c r="D13" s="8">
         <v>12</v>
       </c>
-      <c r="E12" s="36"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="32"/>
-      <c r="B13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="6">
-        <v>4</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="E13" s="30"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="36"/>
+      <c r="B14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6">
+        <v>4</v>
+      </c>
+      <c r="D14" s="6">
         <v>8</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="G13" s="27"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="32"/>
-      <c r="B14" s="6" t="s">
+      <c r="E14" s="33"/>
+      <c r="G14" s="27"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="36"/>
+      <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="7">
-        <v>4</v>
-      </c>
-      <c r="D14" s="8">
+      <c r="C15" s="7">
+        <v>4</v>
+      </c>
+      <c r="D15" s="8">
         <v>16</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="G14" s="27"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="32"/>
-      <c r="B15" s="6" t="s">
+      <c r="E15" s="8"/>
+      <c r="G15" s="27"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="36"/>
+      <c r="B16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="29">
-        <v>4</v>
-      </c>
-      <c r="D15" s="29">
+      <c r="C16" s="29">
+        <v>4</v>
+      </c>
+      <c r="D16" s="29">
         <v>8</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="G15" s="27"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="32"/>
-      <c r="B16" s="6" t="s">
+      <c r="E16" s="14"/>
+      <c r="G16" s="27"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="36"/>
+      <c r="B17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="7">
-        <v>4</v>
-      </c>
-      <c r="D16" s="8">
+      <c r="C17" s="7">
+        <v>4</v>
+      </c>
+      <c r="D17" s="8">
         <v>8</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="G16" s="27"/>
-    </row>
-    <row r="17" spans="1:8" s="25" customFormat="1">
-      <c r="A17" s="32"/>
-      <c r="B17" s="6" t="s">
+      <c r="E17" s="8"/>
+      <c r="G17" s="27"/>
+    </row>
+    <row r="18" spans="1:8" s="25" customFormat="1">
+      <c r="A18" s="36"/>
+      <c r="B18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="29">
-        <v>4</v>
-      </c>
-      <c r="D17" s="29">
+      <c r="C18" s="29">
+        <v>4</v>
+      </c>
+      <c r="D18" s="29">
         <v>10</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="G17" s="27"/>
-    </row>
-    <row r="18" spans="1:8" s="25" customFormat="1">
-      <c r="A18" s="32"/>
-      <c r="B18" s="6" t="s">
+      <c r="E18" s="14"/>
+      <c r="G18" s="27"/>
+    </row>
+    <row r="19" spans="1:8" s="25" customFormat="1">
+      <c r="A19" s="36"/>
+      <c r="B19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="7">
-        <v>4</v>
-      </c>
-      <c r="D18" s="8">
+      <c r="C19" s="7">
+        <v>4</v>
+      </c>
+      <c r="D19" s="8">
         <v>10</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="G18" s="27"/>
-    </row>
-    <row r="19" spans="1:8" s="25" customFormat="1">
-      <c r="C19" s="26"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="30" t="s">
+      <c r="E19" s="8"/>
+      <c r="G19" s="27"/>
+    </row>
+    <row r="20" spans="1:8" s="25" customFormat="1">
+      <c r="C20" s="26"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="30"/>
-      <c r="B21" s="7" t="s">
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="34"/>
+      <c r="B22" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8">
+      <c r="C22" s="8"/>
+      <c r="D22" s="8">
         <v>3</v>
       </c>
-      <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="30"/>
-      <c r="B22" s="4" t="s">
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="34"/>
+      <c r="B23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5">
+      <c r="C23" s="5"/>
+      <c r="D23" s="5">
         <v>6</v>
       </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="30"/>
-      <c r="B23" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8">
-        <v>6</v>
-      </c>
-      <c r="E23" s="7"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:8" s="29" customFormat="1">
-      <c r="A24" s="30"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="4" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5">
@@ -1050,250 +1071,316 @@
       </c>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="30"/>
-      <c r="B25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8">
-        <v>3</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="30"/>
+    <row r="25" spans="1:8" s="29" customFormat="1">
+      <c r="A25" s="34"/>
+      <c r="B25" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5">
+        <v>6</v>
+      </c>
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" s="29" customFormat="1">
+      <c r="A26" s="34"/>
       <c r="B26" s="4" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5">
         <v>6</v>
       </c>
       <c r="E26" s="6"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="30"/>
-      <c r="B27" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8">
-        <v>3</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="30"/>
+    </row>
+    <row r="27" spans="1:8" s="29" customFormat="1">
+      <c r="A27" s="34"/>
+      <c r="B27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5">
+        <v>8</v>
+      </c>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" s="29" customFormat="1">
+      <c r="A28" s="34"/>
       <c r="B28" s="4" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5">
+        <v>20</v>
+      </c>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="34"/>
+      <c r="B29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="C29" s="19"/>
-      <c r="H29" s="2"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8">
+        <v>6</v>
+      </c>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:8" s="29" customFormat="1">
-      <c r="A30" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8">
-        <v>16</v>
-      </c>
-      <c r="E30" s="7"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1">
+      <c r="A30" s="34"/>
+      <c r="B30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5">
+        <v>6</v>
+      </c>
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="34"/>
-      <c r="B31" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5">
-        <v>2</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H31" s="2"/>
+      <c r="B31" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8">
+        <v>3</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="34"/>
-      <c r="B32" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="8">
-        <v>4</v>
-      </c>
-      <c r="D32" s="8">
+      <c r="B32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5">
         <v>6</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="E32" s="6"/>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="34"/>
-      <c r="B33" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="5">
-        <v>4</v>
-      </c>
-      <c r="D33" s="5">
-        <v>6</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="B33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8">
+        <v>3</v>
+      </c>
+      <c r="E33" s="7"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="35"/>
-      <c r="B34" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="8">
-        <v>4</v>
-      </c>
-      <c r="D34" s="8">
-        <v>6</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="A34" s="34"/>
+      <c r="B34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5">
+        <v>12</v>
+      </c>
+      <c r="E34" s="6"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8">
       <c r="C35" s="19"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="B36" s="9" t="s">
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" s="29" customFormat="1">
+      <c r="A36" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8">
+        <v>16</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" customHeight="1">
+      <c r="A37" s="38"/>
+      <c r="B37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5">
+        <v>2</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="38"/>
+      <c r="B38" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="8">
+        <v>4</v>
+      </c>
+      <c r="D38" s="8">
+        <v>6</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="38"/>
+      <c r="B39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="5">
+        <v>4</v>
+      </c>
+      <c r="D39" s="5">
+        <v>6</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="39"/>
+      <c r="B40" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="8">
+        <v>4</v>
+      </c>
+      <c r="D40" s="8">
+        <v>6</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="C41" s="19"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="B42" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C42" s="8">
         <v>8</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D42" s="10">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="B37" s="1"/>
-      <c r="C37" s="19"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="B38" s="9" t="s">
+    <row r="43" spans="1:8">
+      <c r="B43" s="1"/>
+      <c r="C43" s="19"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="B44" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="10">
+      <c r="C44" s="8"/>
+      <c r="D44" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
-      <c r="B40" s="11" t="s">
+    <row r="46" spans="1:8">
+      <c r="B46" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="20">
-        <f>SUM(C2:C36)</f>
+      <c r="C46" s="20">
+        <f>SUM(C2:C42)</f>
         <v>92</v>
       </c>
-      <c r="D40" s="21">
-        <f>SUM(D3:D38)</f>
-        <v>267</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="B41" s="12"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="23"/>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="B42" s="12" t="s">
+      <c r="D46" s="21">
+        <f>SUM(D3:D44)</f>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="B47" s="12"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="23"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="B48" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="22">
-        <f>C40+D40</f>
-        <v>359</v>
-      </c>
-      <c r="D42" s="23"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="B43" s="12"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="23"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="B44" s="15"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="14"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="B45" s="16"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="18"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="24" t="s">
+      <c r="C48" s="22">
+        <f>C46+D46</f>
+        <v>417</v>
+      </c>
+      <c r="D48" s="23"/>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="B49" s="12"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="23"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="B50" s="15"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="14"/>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="B51" s="16"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="18"/>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="1" t="s">
+    <row r="55" spans="1:4">
+      <c r="A55" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B49" s="24" t="s">
+      <c r="B55" s="24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="B50" s="24" t="s">
+    <row r="56" spans="1:4">
+      <c r="B56" s="24" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="B51" s="24" t="s">
+    <row r="57" spans="1:4">
+      <c r="B57" s="24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="B52" s="24" t="s">
+    <row r="58" spans="1:4">
+      <c r="B58" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="B53" s="24" t="s">
+    <row r="59" spans="1:4">
+      <c r="B59" s="24" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" s="1" t="s">
+    <row r="60" spans="1:4">
+      <c r="A60" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="24" t="s">
+      <c r="B60" s="24" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A20:A28"/>
-    <mergeCell ref="A2:A18"/>
-    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A21:A34"/>
+    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="A36:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>